<commit_message>
Complete set up for part obs for ccanada
</commit_message>
<xml_diff>
--- a/pendulum/part_obs_pendulum/part_obs_grav.xlsx
+++ b/pendulum/part_obs_pendulum/part_obs_grav.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sky/Documents/Work Info/Research Assistant/deap_experiments/pendulum/part_obs_pendulum/excel_sheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sky/Documents/Work Info/Research Assistant/deap_experiments/pendulum/part_obs_pendulum/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E451E7-99B6-764E-BBBE-B452D9AAA288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2655602A-2B14-E147-8A88-E221999D7FAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -83,6 +83,21 @@
     <t>add(ang_vel(x1, x3, tan(atan(protectedDiv(x2, x1), ang_vel(x1, x3, add(x1, x2), x3))), x3), tan(tan(x3)))sub(ang_vel(y3, y1, ang_vel(y1, add(add(x1, x2), y1), cos(x1), max(x1, y2)), x2), acos(max(x1, tan(sin(x3))), y3))</t>
   </si>
   <si>
+    <t>protectedDiv(protectedDiv(y3, max(x2, y2)), conditional(x1, sin(max(x2, protectedDiv(y3, cos(protectedDiv(x3, conditional(x1, sin(max(tan(max(sin(acos(x1, y2)), x3)), y3))))))))))</t>
+  </si>
+  <si>
+    <t>add(ang_vel(sub(y1, x1), asin(y2, y2), limit(conditional(y2, y1), add(x2, x2), tan(y1)), ang_vel(x2, max(x3, y3), y3, x3)), acos(atan(max(max(y1, y3), x1), tan(x3)), limit(x1, ang_vel(add(x3, limit(conditional(y2, y1), add(x2, x2), tan(y1))), max(y1, x2), ang_vel(y2, x3, y3, x2), max(y2, y2)), protectedDiv(ang_vel(y2, atan(max(conditional(add(x1, y1), ang_vel(y1, x3, x3, y2)), x1), x2), x3, y3), cos(x3)))))</t>
+  </si>
+  <si>
+    <t>tan(protectedDiv(sin(max(x1, x1)), limit(x3, x3, x1)))</t>
+  </si>
+  <si>
+    <t>sub(asin(y3, y3), ang_vel(y1, y3, sin(atan(ang_vel(atan(y1, y3), x2, ang_vel(add(protectedDiv(x1, y3), limit(x2, y2, x2)), x2, asin(x1, x3), cos(atan(cos(x2), sin(x1)))), cos(atan(cos(asin(atan(y3, y1), limit(x3, x1, y2))), sin(x1)))), y1)), sin(conditional(x2, x2))))</t>
+  </si>
+  <si>
+    <t>limit(tan(protectedDiv(add(y2, x3), x1)), ang_vel(y3, y2, max(acos(y1, x1), sub(x3, limit(y3, y2, x3))), x3), acos(protectedDiv(add(x1, x1), max(x3, ang_vel(x2, x2, x1, y1))), protectedDiv(acos(add(sin(x1), protectedDiv(x1, sin(asin(x1, y1)))), y2), x3)))</t>
+  </si>
+  <si>
     <t>sub(ang_vel(y3, y1, ang_vel(y1, add(add(x1, x2), y1), cos(x1), max(x1, y2)), x2), acos(max(x1, tan(sin(x3))), y3))</t>
   </si>
   <si>
@@ -111,21 +126,6 @@
   </si>
   <si>
     <t>conditional(acos(x3, y3), sub(atan(sub(y2, x3), x3), sub(x2, x1)))</t>
-  </si>
-  <si>
-    <t>protectedDiv(protectedDiv(y3, max(x2, y2)), conditional(x1, sin(max(x2, protectedDiv(y3, cos(protectedDiv(x3, conditional(x1, sin(max(tan(max(sin(acos(x1, y2)), x3)), y3))))))))))</t>
-  </si>
-  <si>
-    <t>add(ang_vel(sub(y1, x1), asin(y2, y2), limit(conditional(y2, y1), add(x2, x2), tan(y1)), ang_vel(x2, max(x3, y3), y3, x3)), acos(atan(max(max(y1, y3), x1), tan(x3)), limit(x1, ang_vel(add(x3, limit(conditional(y2, y1), add(x2, x2), tan(y1))), max(y1, x2), ang_vel(y2, x3, y3, x2), max(y2, y2)), protectedDiv(ang_vel(y2, atan(max(conditional(add(x1, y1), ang_vel(y1, x3, x3, y2)), x1), x2), x3, y3), cos(x3)))))</t>
-  </si>
-  <si>
-    <t>tan(protectedDiv(sin(max(x1, x1)), limit(x3, x3, x1)))</t>
-  </si>
-  <si>
-    <t>sub(asin(y3, y3), ang_vel(y1, y3, sin(atan(ang_vel(atan(y1, y3), x2, ang_vel(add(protectedDiv(x1, y3), limit(x2, y2, x2)), x2, asin(x1, x3), cos(atan(cos(x2), sin(x1)))), cos(atan(cos(asin(atan(y3, y1), limit(x3, x1, y2))), sin(x1)))), y1)), sin(conditional(x2, x2))))</t>
-  </si>
-  <si>
-    <t>limit(tan(protectedDiv(add(y2, x3), x1)), ang_vel(y3, y2, max(acos(y1, x1), sub(x3, limit(y3, y2, x3))), x3), acos(protectedDiv(add(x1, x1), max(x3, ang_vel(x2, x2, x1, y1))), protectedDiv(acos(add(sin(x1), protectedDiv(x1, sin(asin(x1, y1)))), y2), x3)))</t>
   </si>
   <si>
     <t>g=15</t>
@@ -228,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -244,7 +244,6 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -277,34 +276,23 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:endParaRPr lang="en-CA"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
           <a:noFill/>
+          <a:prstDash val="solid"/>
         </a:ln>
-        <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -331,9 +319,9 @@
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
+              <a:prstDash val="solid"/>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -455,7 +443,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-6FA0-5440-AD65-7C9683DF3ADE}"/>
+              <c16:uniqueId val="{00000000-E3A9-6645-BAB7-8BA9C8FBC9E9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -478,9 +466,9 @@
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
+              <a:prstDash val="solid"/>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -602,7 +590,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-6FA0-5440-AD65-7C9683DF3ADE}"/>
+              <c16:uniqueId val="{00000001-E3A9-6645-BAB7-8BA9C8FBC9E9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -625,9 +613,9 @@
               <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
+              <a:prstDash val="solid"/>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -749,7 +737,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-6FA0-5440-AD65-7C9683DF3ADE}"/>
+              <c16:uniqueId val="{00000002-E3A9-6645-BAB7-8BA9C8FBC9E9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -772,9 +760,9 @@
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
+              <a:prstDash val="solid"/>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -896,7 +884,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-6FA0-5440-AD65-7C9683DF3ADE}"/>
+              <c16:uniqueId val="{00000003-E3A9-6645-BAB7-8BA9C8FBC9E9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -919,9 +907,9 @@
               <a:solidFill>
                 <a:schemeClr val="accent5"/>
               </a:solidFill>
+              <a:prstDash val="solid"/>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -1043,7 +1031,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-6FA0-5440-AD65-7C9683DF3ADE}"/>
+              <c16:uniqueId val="{00000004-E3A9-6645-BAB7-8BA9C8FBC9E9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1066,9 +1054,9 @@
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
               </a:solidFill>
+              <a:prstDash val="solid"/>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -1190,7 +1178,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-6FA0-5440-AD65-7C9683DF3ADE}"/>
+              <c16:uniqueId val="{00000005-E3A9-6645-BAB7-8BA9C8FBC9E9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1226,16 +1214,16 @@
                 <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
+            <a:prstDash val="solid"/>
             <a:round/>
           </a:ln>
-          <a:effectLst/>
         </c:spPr>
         <c:txPr>
           <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1273,9 +1261,9 @@
                   <a:lumOff val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:prstDash val="solid"/>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
         <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
@@ -1286,15 +1274,15 @@
           <a:noFill/>
           <a:ln>
             <a:noFill/>
+            <a:prstDash val="solid"/>
           </a:ln>
-          <a:effectLst/>
         </c:spPr>
         <c:txPr>
           <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1313,13 +1301,6 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
@@ -1328,15 +1309,15 @@
         <a:noFill/>
         <a:ln>
           <a:noFill/>
+          <a:prstDash val="solid"/>
         </a:ln>
-        <a:effectLst/>
       </c:spPr>
       <c:txPr>
         <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1354,13 +1335,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -1374,582 +1348,16 @@
           <a:lumOff val="85000"/>
         </a:schemeClr>
       </a:solidFill>
+      <a:prstDash val="solid"/>
       <a:round/>
     </a:ln>
-    <a:effectLst/>
   </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
-</file>
-
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1972,7 +1380,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3C3FCFD-1DC2-6129-F9BA-C10D992363AF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2281,11 +1689,9 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:R52"/>
+  <dimension ref="A1:R38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T37" sqref="T37"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3145,7 +2551,7 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B17" s="9">
         <v>-806.07</v>
@@ -3198,7 +2604,7 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B18" s="9">
         <v>-2448.34</v>
@@ -3251,7 +2657,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B19" s="9">
         <v>-3626.02</v>
@@ -3304,7 +2710,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B20" s="9">
         <v>-1286.81</v>
@@ -3357,7 +2763,7 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B21" s="9">
         <v>-3122.85</v>
@@ -3410,7 +2816,7 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B22" s="6">
         <v>-2084.5300000000002</v>
@@ -3463,7 +2869,7 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B23" s="6">
         <v>-1930.79</v>
@@ -3516,7 +2922,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B24" s="6">
         <v>-123.96</v>
@@ -3569,7 +2975,7 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B25" s="6">
         <v>-1601.63</v>
@@ -3622,7 +3028,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B26" s="6">
         <v>-1233.8499999999999</v>
@@ -3675,7 +3081,7 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B27" s="7">
         <v>-3720.39</v>
@@ -3728,7 +3134,7 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B28" s="7">
         <v>-3648.68</v>
@@ -3781,7 +3187,7 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B29" s="7">
         <v>-3668.77</v>
@@ -3834,7 +3240,7 @@
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B30" s="7">
         <v>-3578.01</v>
@@ -3887,7 +3293,7 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B31" s="7">
         <v>-3679.36</v>
@@ -3993,67 +3399,67 @@
         <v>31</v>
       </c>
       <c r="B33" s="2">
-        <f>AVERAGE(B27:B31)</f>
+        <f t="shared" ref="B33:Q33" si="0">AVERAGE(B27:B31)</f>
         <v>-3659.0419999999999</v>
       </c>
       <c r="C33" s="2">
-        <f>AVERAGE(C27:C31)</f>
+        <f t="shared" si="0"/>
         <v>-3620.4840000000004</v>
       </c>
       <c r="D33" s="2">
-        <f>AVERAGE(D27:D31)</f>
+        <f t="shared" si="0"/>
         <v>-3491.1019999999999</v>
       </c>
       <c r="E33" s="2">
-        <f>AVERAGE(E27:E31)</f>
+        <f t="shared" si="0"/>
         <v>-3457.3199999999997</v>
       </c>
       <c r="F33" s="2">
-        <f>AVERAGE(F27:F31)</f>
+        <f t="shared" si="0"/>
         <v>-3519.1600000000008</v>
       </c>
       <c r="G33" s="2">
-        <f>AVERAGE(G27:G31)</f>
+        <f t="shared" si="0"/>
         <v>-3438.8919999999998</v>
       </c>
       <c r="H33" s="2">
-        <f>AVERAGE(H27:H31)</f>
+        <f t="shared" si="0"/>
         <v>-3332.3679999999999</v>
       </c>
       <c r="I33" s="2">
-        <f>AVERAGE(I27:I31)</f>
+        <f t="shared" si="0"/>
         <v>-3236.8399999999997</v>
       </c>
       <c r="J33" s="2">
-        <f>AVERAGE(J27:J31)</f>
+        <f t="shared" si="0"/>
         <v>-3004.98</v>
       </c>
       <c r="K33" s="2">
-        <f>AVERAGE(K27:K31)</f>
+        <f t="shared" si="0"/>
         <v>-2848.1460000000002</v>
       </c>
       <c r="L33" s="2">
-        <f>AVERAGE(L27:L31)</f>
+        <f t="shared" si="0"/>
         <v>-2678.8480000000004</v>
       </c>
       <c r="M33" s="2">
-        <f>AVERAGE(M27:M31)</f>
+        <f t="shared" si="0"/>
         <v>-2479.1040000000003</v>
       </c>
       <c r="N33" s="2">
-        <f>AVERAGE(N27:N31)</f>
+        <f t="shared" si="0"/>
         <v>-2141.2820000000002</v>
       </c>
       <c r="O33" s="2">
-        <f>AVERAGE(O27:O31)</f>
+        <f t="shared" si="0"/>
         <v>-1427.8720000000001</v>
       </c>
       <c r="P33" s="2">
-        <f>AVERAGE(P27:P31)</f>
+        <f t="shared" si="0"/>
         <v>-2202.0700000000002</v>
       </c>
       <c r="Q33" s="2">
-        <f>AVERAGE(Q27:Q31)</f>
+        <f t="shared" si="0"/>
         <v>-2509.5320000000002</v>
       </c>
     </row>
@@ -4062,67 +3468,67 @@
         <v>32</v>
       </c>
       <c r="B34" s="2">
-        <f>AVERAGE(B22:B26)</f>
+        <f t="shared" ref="B34:Q34" si="1">AVERAGE(B22:B26)</f>
         <v>-1394.952</v>
       </c>
       <c r="C34" s="2">
-        <f>AVERAGE(C22:C26)</f>
+        <f t="shared" si="1"/>
         <v>-1604.4180000000001</v>
       </c>
       <c r="D34" s="2">
-        <f>AVERAGE(D22:D26)</f>
+        <f t="shared" si="1"/>
         <v>-1712.5</v>
       </c>
       <c r="E34" s="2">
-        <f>AVERAGE(E22:E26)</f>
+        <f t="shared" si="1"/>
         <v>-1811.98</v>
       </c>
       <c r="F34" s="2">
-        <f>AVERAGE(F22:F26)</f>
+        <f t="shared" si="1"/>
         <v>-2008.4979999999996</v>
       </c>
       <c r="G34" s="2">
-        <f>AVERAGE(G22:G26)</f>
+        <f t="shared" si="1"/>
         <v>-2205.7419999999997</v>
       </c>
       <c r="H34" s="2">
-        <f>AVERAGE(H22:H26)</f>
+        <f t="shared" si="1"/>
         <v>-2654.68</v>
       </c>
       <c r="I34" s="2">
-        <f>AVERAGE(I22:I26)</f>
+        <f t="shared" si="1"/>
         <v>-2612.1940000000004</v>
       </c>
       <c r="J34" s="2">
-        <f>AVERAGE(J22:J26)</f>
+        <f t="shared" si="1"/>
         <v>-2433.0360000000001</v>
       </c>
       <c r="K34" s="2">
-        <f>AVERAGE(K22:K26)</f>
+        <f t="shared" si="1"/>
         <v>-2293.4960000000001</v>
       </c>
       <c r="L34" s="2">
-        <f>AVERAGE(L22:L26)</f>
+        <f t="shared" si="1"/>
         <v>-2107.1819999999998</v>
       </c>
       <c r="M34" s="2">
-        <f>AVERAGE(M22:M26)</f>
+        <f t="shared" si="1"/>
         <v>-1676.2579999999998</v>
       </c>
       <c r="N34" s="2">
-        <f>AVERAGE(N22:N26)</f>
+        <f t="shared" si="1"/>
         <v>-777.75400000000002</v>
       </c>
       <c r="O34" s="2">
-        <f>AVERAGE(O22:O26)</f>
+        <f t="shared" si="1"/>
         <v>-1923.9779999999998</v>
       </c>
       <c r="P34" s="2">
-        <f>AVERAGE(P22:P26)</f>
+        <f t="shared" si="1"/>
         <v>-2238.7820000000002</v>
       </c>
       <c r="Q34" s="2">
-        <f>AVERAGE(Q22:Q26)</f>
+        <f t="shared" si="1"/>
         <v>-2375.4300000000003</v>
       </c>
     </row>
@@ -4131,67 +3537,67 @@
         <v>33</v>
       </c>
       <c r="B35" s="2">
-        <f>AVERAGE(B17:B21)</f>
+        <f t="shared" ref="B35:Q35" si="2">AVERAGE(B17:B21)</f>
         <v>-2258.018</v>
       </c>
       <c r="C35" s="2">
-        <f>AVERAGE(C17:C21)</f>
+        <f t="shared" si="2"/>
         <v>-2252.596</v>
       </c>
       <c r="D35" s="2">
-        <f>AVERAGE(D17:D21)</f>
+        <f t="shared" si="2"/>
         <v>-2476.3839999999996</v>
       </c>
       <c r="E35" s="2">
-        <f>AVERAGE(E17:E21)</f>
+        <f t="shared" si="2"/>
         <v>-2634.694</v>
       </c>
       <c r="F35" s="2">
-        <f>AVERAGE(F17:F21)</f>
+        <f t="shared" si="2"/>
         <v>-2621.7359999999999</v>
       </c>
       <c r="G35" s="2">
-        <f>AVERAGE(G17:G21)</f>
+        <f t="shared" si="2"/>
         <v>-2532.2080000000001</v>
       </c>
       <c r="H35" s="2">
-        <f>AVERAGE(H17:H21)</f>
+        <f t="shared" si="2"/>
         <v>-2576.2460000000001</v>
       </c>
       <c r="I35" s="2">
-        <f>AVERAGE(I17:I21)</f>
+        <f t="shared" si="2"/>
         <v>-2487.232</v>
       </c>
       <c r="J35" s="2">
-        <f>AVERAGE(J17:J21)</f>
+        <f t="shared" si="2"/>
         <v>-2243.576</v>
       </c>
       <c r="K35" s="2">
-        <f>AVERAGE(K17:K21)</f>
+        <f t="shared" si="2"/>
         <v>-2070.6800000000003</v>
       </c>
       <c r="L35" s="2">
-        <f>AVERAGE(L17:L21)</f>
+        <f t="shared" si="2"/>
         <v>-1922.33</v>
       </c>
       <c r="M35" s="2">
-        <f>AVERAGE(M17:M21)</f>
+        <f t="shared" si="2"/>
         <v>-1497.7660000000001</v>
       </c>
       <c r="N35" s="2">
-        <f>AVERAGE(N17:N21)</f>
+        <f t="shared" si="2"/>
         <v>-806.13599999999997</v>
       </c>
       <c r="O35" s="2">
-        <f>AVERAGE(O17:O21)</f>
+        <f t="shared" si="2"/>
         <v>-2217.4219999999996</v>
       </c>
       <c r="P35" s="2">
-        <f>AVERAGE(P17:P21)</f>
+        <f t="shared" si="2"/>
         <v>-2458.4399999999996</v>
       </c>
       <c r="Q35" s="2">
-        <f>AVERAGE(Q17:Q21)</f>
+        <f t="shared" si="2"/>
         <v>-2600.4839999999999</v>
       </c>
     </row>
@@ -4200,67 +3606,67 @@
         <v>34</v>
       </c>
       <c r="B36" s="2">
-        <f>AVERAGE(B12:B16)</f>
+        <f t="shared" ref="B36:Q36" si="3">AVERAGE(B12:B16)</f>
         <v>-1882.7060000000001</v>
       </c>
       <c r="C36" s="2">
-        <f>AVERAGE(C12:C16)</f>
+        <f t="shared" si="3"/>
         <v>-2169.902</v>
       </c>
       <c r="D36" s="2">
-        <f>AVERAGE(D12:D16)</f>
+        <f t="shared" si="3"/>
         <v>-2197.8419999999996</v>
       </c>
       <c r="E36" s="2">
-        <f>AVERAGE(E12:E16)</f>
+        <f t="shared" si="3"/>
         <v>-2176.0720000000001</v>
       </c>
       <c r="F36" s="2">
-        <f>AVERAGE(F12:F16)</f>
+        <f t="shared" si="3"/>
         <v>-2133.9379999999996</v>
       </c>
       <c r="G36" s="2">
-        <f>AVERAGE(G12:G16)</f>
+        <f t="shared" si="3"/>
         <v>-2148.14</v>
       </c>
       <c r="H36" s="2">
-        <f>AVERAGE(H12:H16)</f>
+        <f t="shared" si="3"/>
         <v>-2177.5239999999999</v>
       </c>
       <c r="I36" s="2">
-        <f>AVERAGE(I12:I16)</f>
+        <f t="shared" si="3"/>
         <v>-1924.1560000000002</v>
       </c>
       <c r="J36" s="2">
-        <f>AVERAGE(J12:J16)</f>
+        <f t="shared" si="3"/>
         <v>-1707.4360000000001</v>
       </c>
       <c r="K36" s="2">
-        <f>AVERAGE(K12:K16)</f>
+        <f t="shared" si="3"/>
         <v>-1533.5579999999998</v>
       </c>
       <c r="L36" s="2">
-        <f>AVERAGE(L12:L16)</f>
+        <f t="shared" si="3"/>
         <v>-908.87200000000007</v>
       </c>
       <c r="M36" s="2">
-        <f>AVERAGE(M12:M16)</f>
+        <f t="shared" si="3"/>
         <v>-1860.4720000000002</v>
       </c>
       <c r="N36" s="2">
-        <f>AVERAGE(N12:N16)</f>
+        <f t="shared" si="3"/>
         <v>-2041.8919999999998</v>
       </c>
       <c r="O36" s="2">
-        <f>AVERAGE(O12:O16)</f>
+        <f t="shared" si="3"/>
         <v>-2441.402</v>
       </c>
       <c r="P36" s="2">
-        <f>AVERAGE(P12:P16)</f>
+        <f t="shared" si="3"/>
         <v>-2592.2300000000005</v>
       </c>
       <c r="Q36" s="2">
-        <f>AVERAGE(Q12:Q16)</f>
+        <f t="shared" si="3"/>
         <v>-2739.7260000000001</v>
       </c>
     </row>
@@ -4269,67 +3675,67 @@
         <v>35</v>
       </c>
       <c r="B37" s="2">
-        <f>AVERAGE(B7:B11)</f>
+        <f t="shared" ref="B37:Q37" si="4">AVERAGE(B7:B11)</f>
         <v>-2037.2280000000003</v>
       </c>
       <c r="C37" s="2">
-        <f>AVERAGE(C7:C11)</f>
+        <f t="shared" si="4"/>
         <v>-1990.836</v>
       </c>
       <c r="D37" s="2">
-        <f>AVERAGE(D7:D11)</f>
+        <f t="shared" si="4"/>
         <v>-2011.7360000000001</v>
       </c>
       <c r="E37" s="2">
-        <f>AVERAGE(E7:E11)</f>
+        <f t="shared" si="4"/>
         <v>-1923.364</v>
       </c>
       <c r="F37" s="2">
-        <f>AVERAGE(F7:F11)</f>
+        <f t="shared" si="4"/>
         <v>-2035.5100000000002</v>
       </c>
       <c r="G37" s="2">
-        <f>AVERAGE(G7:G11)</f>
+        <f t="shared" si="4"/>
         <v>-1895.4720000000002</v>
       </c>
       <c r="H37" s="2">
-        <f>AVERAGE(H7:H11)</f>
+        <f t="shared" si="4"/>
         <v>-2030.848</v>
       </c>
       <c r="I37" s="2">
-        <f>AVERAGE(I7:I11)</f>
+        <f t="shared" si="4"/>
         <v>-1960.184</v>
       </c>
       <c r="J37" s="2">
-        <f>AVERAGE(J7:J11)</f>
+        <f t="shared" si="4"/>
         <v>-1640.4099999999999</v>
       </c>
       <c r="K37" s="2">
-        <f>AVERAGE(K7:K11)</f>
+        <f t="shared" si="4"/>
         <v>-1123.508</v>
       </c>
       <c r="L37" s="2">
-        <f>AVERAGE(L7:L11)</f>
+        <f t="shared" si="4"/>
         <v>-1370.24</v>
       </c>
       <c r="M37" s="2">
-        <f>AVERAGE(M7:M11)</f>
+        <f t="shared" si="4"/>
         <v>-1938.0319999999999</v>
       </c>
       <c r="N37" s="2">
-        <f>AVERAGE(N7:N11)</f>
+        <f t="shared" si="4"/>
         <v>-2390.9960000000001</v>
       </c>
       <c r="O37" s="2">
-        <f>AVERAGE(O7:O11)</f>
+        <f t="shared" si="4"/>
         <v>-2553.4679999999998</v>
       </c>
       <c r="P37" s="2">
-        <f>AVERAGE(P7:P11)</f>
+        <f t="shared" si="4"/>
         <v>-2693.2079999999996</v>
       </c>
       <c r="Q37" s="2">
-        <f>AVERAGE(Q7:Q11)</f>
+        <f t="shared" si="4"/>
         <v>-2751.3679999999999</v>
       </c>
     </row>
@@ -4338,186 +3744,69 @@
         <v>36</v>
       </c>
       <c r="B38" s="2">
-        <f>AVERAGE(B2:B6)</f>
+        <f t="shared" ref="B38:Q38" si="5">AVERAGE(B2:B6)</f>
         <v>-753.33799999999997</v>
       </c>
       <c r="C38" s="2">
-        <f>AVERAGE(C2:C6)</f>
+        <f t="shared" si="5"/>
         <v>-881.42400000000021</v>
       </c>
       <c r="D38" s="2">
-        <f>AVERAGE(D2:D6)</f>
+        <f t="shared" si="5"/>
         <v>-796.74199999999996</v>
       </c>
       <c r="E38" s="2">
-        <f>AVERAGE(E2:E6)</f>
+        <f t="shared" si="5"/>
         <v>-846.59199999999998</v>
       </c>
       <c r="F38" s="2">
-        <f>AVERAGE(F2:F6)</f>
+        <f t="shared" si="5"/>
         <v>-996.06999999999994</v>
       </c>
       <c r="G38" s="2">
-        <f>AVERAGE(G2:G6)</f>
+        <f t="shared" si="5"/>
         <v>-1085.962</v>
       </c>
       <c r="H38" s="2">
-        <f>AVERAGE(H2:H6)</f>
+        <f t="shared" si="5"/>
         <v>-1169.8480000000002</v>
       </c>
       <c r="I38" s="2">
-        <f>AVERAGE(I2:I6)</f>
+        <f t="shared" si="5"/>
         <v>-1028.5279999999998</v>
       </c>
       <c r="J38" s="2">
-        <f>AVERAGE(J2:J6)</f>
+        <f t="shared" si="5"/>
         <v>-587.548</v>
       </c>
       <c r="K38" s="2">
-        <f>AVERAGE(K2:K6)</f>
+        <f t="shared" si="5"/>
         <v>-933.92600000000004</v>
       </c>
       <c r="L38" s="2">
-        <f>AVERAGE(L2:L6)</f>
+        <f t="shared" si="5"/>
         <v>-1392.2080000000001</v>
       </c>
       <c r="M38" s="2">
-        <f>AVERAGE(M2:M6)</f>
+        <f t="shared" si="5"/>
         <v>-1782.846</v>
       </c>
       <c r="N38" s="2">
-        <f>AVERAGE(N2:N6)</f>
+        <f t="shared" si="5"/>
         <v>-2283.7460000000001</v>
       </c>
       <c r="O38" s="2">
-        <f>AVERAGE(O2:O6)</f>
+        <f t="shared" si="5"/>
         <v>-2422.9459999999999</v>
       </c>
       <c r="P38" s="2">
-        <f>AVERAGE(P2:P6)</f>
+        <f t="shared" si="5"/>
         <v>-2559.81</v>
       </c>
       <c r="Q38" s="2">
-        <f>AVERAGE(Q2:Q6)</f>
+        <f t="shared" si="5"/>
         <v>-2672.348</v>
       </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="11"/>
-      <c r="B47" s="11"/>
-      <c r="C47" s="11"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="11"/>
-      <c r="F47" s="11"/>
-      <c r="G47" s="11"/>
-      <c r="H47" s="11"/>
-      <c r="I47" s="11"/>
-      <c r="J47" s="11"/>
-      <c r="K47" s="11"/>
-      <c r="L47" s="11"/>
-      <c r="M47" s="11"/>
-      <c r="N47" s="11"/>
-      <c r="O47" s="11"/>
-      <c r="P47" s="11"/>
-      <c r="Q47" s="11"/>
-    </row>
-    <row r="48" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="11"/>
-      <c r="B48" s="11"/>
-      <c r="C48" s="11"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="11"/>
-      <c r="F48" s="11"/>
-      <c r="G48" s="11"/>
-      <c r="H48" s="11"/>
-      <c r="I48" s="11"/>
-      <c r="J48" s="11"/>
-      <c r="K48" s="11"/>
-      <c r="L48" s="11"/>
-      <c r="M48" s="11"/>
-      <c r="N48" s="11"/>
-      <c r="O48" s="11"/>
-      <c r="P48" s="11"/>
-      <c r="Q48" s="11"/>
-    </row>
-    <row r="49" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="11"/>
-      <c r="B49" s="11"/>
-      <c r="C49" s="11"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="11"/>
-      <c r="F49" s="11"/>
-      <c r="G49" s="11"/>
-      <c r="H49" s="11"/>
-      <c r="I49" s="11"/>
-      <c r="J49" s="11"/>
-      <c r="K49" s="11"/>
-      <c r="L49" s="11"/>
-      <c r="M49" s="11"/>
-      <c r="N49" s="11"/>
-      <c r="O49" s="11"/>
-      <c r="P49" s="11"/>
-      <c r="Q49" s="11"/>
-    </row>
-    <row r="50" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="11"/>
-      <c r="B50" s="11"/>
-      <c r="C50" s="11"/>
-      <c r="D50" s="11"/>
-      <c r="E50" s="11"/>
-      <c r="F50" s="11"/>
-      <c r="G50" s="11"/>
-      <c r="H50" s="11"/>
-      <c r="I50" s="11"/>
-      <c r="J50" s="11"/>
-      <c r="K50" s="11"/>
-      <c r="L50" s="11"/>
-      <c r="M50" s="11"/>
-      <c r="N50" s="11"/>
-      <c r="O50" s="11"/>
-      <c r="P50" s="11"/>
-      <c r="Q50" s="11"/>
-    </row>
-    <row r="51" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="11"/>
-      <c r="B51" s="11"/>
-      <c r="C51" s="11"/>
-      <c r="D51" s="11"/>
-      <c r="E51" s="11"/>
-      <c r="F51" s="11"/>
-      <c r="G51" s="11"/>
-      <c r="H51" s="11"/>
-      <c r="I51" s="11"/>
-      <c r="J51" s="11"/>
-      <c r="K51" s="11"/>
-      <c r="L51" s="11"/>
-      <c r="M51" s="11"/>
-      <c r="N51" s="11"/>
-      <c r="O51" s="11"/>
-      <c r="P51" s="11"/>
-      <c r="Q51" s="11"/>
-    </row>
-    <row r="52" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="11"/>
-      <c r="B52" s="11"/>
-      <c r="C52" s="11"/>
-      <c r="D52" s="11"/>
-      <c r="E52" s="11"/>
-      <c r="F52" s="11"/>
-      <c r="G52" s="11"/>
-      <c r="H52" s="11"/>
-      <c r="I52" s="11"/>
-      <c r="J52" s="11"/>
-      <c r="K52" s="11"/>
-      <c r="L52" s="11"/>
-      <c r="M52" s="11"/>
-      <c r="N52" s="11"/>
-      <c r="O52" s="11"/>
-      <c r="P52" s="11"/>
-      <c r="Q52" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>